<commit_message>
edit order and some documentation
</commit_message>
<xml_diff>
--- a/documentation/Specification.xlsx
+++ b/documentation/Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Documents\github\final_project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{232A6431-6421-461A-A687-F8533506471F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15730483-EEAC-49B9-9B60-9C3AEFBF6DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8475" yWindow="2475" windowWidth="23385" windowHeight="11385" xr2:uid="{DBD8C040-893C-43FC-A26A-357F42B1B029}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBD8C040-893C-43FC-A26A-357F42B1B029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>module</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>(admin) user can add/remove new/old users</t>
+  </si>
+  <si>
+    <t>user may send message with no text and with images</t>
+  </si>
+  <si>
+    <t>user may send message with only images</t>
   </si>
 </sst>
 </file>
@@ -364,9 +370,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,12 +379,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -399,9 +396,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -410,23 +404,35 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,10 +748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058E5FB7-927E-4A02-B05D-CC87DD6D6C98}">
-  <dimension ref="A2:D80"/>
+  <dimension ref="A2:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,744 +784,772 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6">
+      <c r="A5" s="24"/>
+      <c r="B5" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6">
+      <c r="A6" s="24"/>
+      <c r="B6" s="5">
         <v>1.2</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6">
+      <c r="A7" s="24"/>
+      <c r="B7" s="5">
         <v>1.3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6">
+      <c r="A8" s="24"/>
+      <c r="B8" s="5">
         <v>1.4</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6">
+      <c r="A9" s="24"/>
+      <c r="B9" s="5">
         <v>1.5</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6">
+      <c r="A10" s="24"/>
+      <c r="B10" s="5">
         <v>1.6</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6">
+      <c r="A11" s="24"/>
+      <c r="B11" s="5">
         <v>1.7</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6">
+      <c r="A12" s="24"/>
+      <c r="B12" s="5">
         <v>1.8</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8">
+      <c r="A14" s="24"/>
+      <c r="B14" s="7">
         <v>2.1</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8">
+      <c r="A15" s="24"/>
+      <c r="B15" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="7">
         <v>3</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="7">
         <v>3.1</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="8">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="7">
         <v>3.2</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="7">
         <v>4</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="8">
+      <c r="A20" s="24"/>
+      <c r="B20" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="8">
+      <c r="A21" s="24"/>
+      <c r="B21" s="7">
         <v>4.2</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8">
+      <c r="A22" s="24"/>
+      <c r="B22" s="7">
         <v>4.3</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="8">
+      <c r="A23" s="24"/>
+      <c r="B23" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="8">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="7">
         <v>5</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="8">
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="7">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="7" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="8">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="7">
         <v>5.2</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="7" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="8">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="7">
         <v>5.3</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="7" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="8">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="7">
         <v>6</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="8">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="7">
         <v>7</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="8">
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="7">
         <v>8</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="8">
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="7">
         <v>9</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="8">
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="7">
         <v>10</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="8">
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="7">
         <v>11</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9" t="s">
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="7" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="7" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="7" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="7" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="7" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B46" s="10">
         <v>4</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C46" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="13">
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="10">
         <v>5</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C47" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13">
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="10">
         <v>6</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C48" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:4" ht="225" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="13">
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="10">
         <v>7</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C49" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="13">
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
+      <c r="B50" s="10">
         <v>8</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C50" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D50" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="13">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="26"/>
+      <c r="B51" s="10">
         <v>8.1</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="15" t="s">
+      <c r="C51" s="11"/>
+      <c r="D51" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="13">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="10">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="15" t="s">
+      <c r="C52" s="11"/>
+      <c r="D52" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="13">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="15" t="s">
+      <c r="C53" s="11"/>
+      <c r="D53" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="13">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
+      <c r="B54" s="10">
         <v>8.4</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="15" t="s">
+      <c r="C54" s="11"/>
+      <c r="D54" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="13">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
+      <c r="B55" s="10">
         <v>8.5</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="15" t="s">
+      <c r="C55" s="11"/>
+      <c r="D55" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18"/>
-    </row>
-    <row r="55" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="15"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B57" s="16">
         <v>9</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C57" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="22"/>
-    </row>
-    <row r="56" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="20">
+      <c r="D57" s="18"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="27"/>
+      <c r="B58" s="16">
         <v>10</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C58" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="22"/>
-    </row>
-    <row r="57" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="20">
+      <c r="D58" s="18"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="27"/>
+      <c r="B59" s="16">
         <v>11</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C59" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="22"/>
-    </row>
-    <row r="58" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="20">
+      <c r="D59" s="18"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="27"/>
+      <c r="B60" s="16">
         <v>12</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C60" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="22"/>
-    </row>
-    <row r="59" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20">
+      <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="27"/>
+      <c r="B61" s="16">
         <v>13</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C61" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="22"/>
-    </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="20">
+      <c r="D61" s="18"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="27"/>
+      <c r="B62" s="16">
         <v>14</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C62" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="22"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="18"/>
-    </row>
-    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="15"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="24">
+      <c r="B64" s="19">
         <v>1</v>
       </c>
-      <c r="C62" s="25" t="s">
+      <c r="C64" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="26"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="24">
+      <c r="D64" s="21"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="28"/>
+      <c r="B65" s="19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="26" t="s">
+      <c r="C65" s="20"/>
+      <c r="D65" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="28"/>
+      <c r="B66" s="19">
         <v>1.2</v>
       </c>
-      <c r="C64" s="25"/>
-      <c r="D64" s="26" t="s">
+      <c r="C66" s="20"/>
+      <c r="D66" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="24">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="28"/>
+      <c r="B67" s="19">
         <v>1.3</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="26" t="s">
+      <c r="C67" s="20"/>
+      <c r="D67" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="26" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="28"/>
+      <c r="B68" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="25" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="28"/>
+      <c r="B69" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="28"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D67" s="26"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="26" t="s">
+      <c r="D70" s="21"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="28"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="27" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="28"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="B70" s="24">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="28"/>
+      <c r="B73" s="19">
         <v>2</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C73" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D70" s="26"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="26" t="s">
+      <c r="D73" s="21"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="28"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="26" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="26" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="28"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="24">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="28"/>
+      <c r="B77" s="19">
         <v>3</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C77" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D74" s="26"/>
-    </row>
-    <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25" t="s">
+      <c r="D77" s="21"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="28"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="24">
+      <c r="D78" s="21"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="28"/>
+      <c r="B79" s="19">
         <v>4</v>
       </c>
-      <c r="C76" s="25" t="s">
+      <c r="C79" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D76" s="26"/>
-    </row>
-    <row r="77" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
-      <c r="B77" s="24">
+      <c r="D79" s="21"/>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="28"/>
+      <c r="B80" s="19">
         <v>5</v>
       </c>
-      <c r="C77" s="28" t="s">
+      <c r="C80" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D77" s="26" t="s">
+      <c r="D80" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="26" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="28"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="26" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="28"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="26"/>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="28"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A4:A42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A62:A80"/>
+    <mergeCell ref="A4:A44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="A64:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>